<commit_message>
Updated hsp_streamlit.py to version 1.0.2.  Modified Excel Files (Materials/Material Types/Suppliers and Default_Materials path).  Modified Title/Section styles (color, etc.).
</commit_message>
<xml_diff>
--- a/data/target_materials/Suppliers.xlsx
+++ b/data/target_materials/Suppliers.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sammo\Projects\HansenSolubilityParameters\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sammo\Projects\HSP\data\target_materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72DFB27-44EA-4A81-B6A0-3587B7A35583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5491C2-3E72-4A97-8F68-746C5AAC0570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Covestro" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkema" sheetId="5" r:id="rId1"/>
     <sheet name="BASF" sheetId="2" r:id="rId2"/>
-    <sheet name="Dow_RohmHaas" sheetId="3" r:id="rId3"/>
-    <sheet name="Evonik" sheetId="4" r:id="rId4"/>
-    <sheet name="Arkema" sheetId="5" r:id="rId5"/>
-    <sheet name="Eastman" sheetId="6" r:id="rId6"/>
+    <sheet name="Covestro" sheetId="1" r:id="rId3"/>
+    <sheet name="Dow" sheetId="3" r:id="rId4"/>
+    <sheet name="Eastman" sheetId="6" r:id="rId5"/>
+    <sheet name="Evonik" sheetId="4" r:id="rId6"/>
     <sheet name="Generic_CASE" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -28,12 +28,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="92">
   <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
     <t>Type / Application</t>
   </si>
   <si>
@@ -302,6 +296,12 @@
   </si>
   <si>
     <t>Higher crosslink density epoxy precursor.</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Supplier</t>
   </si>
 </sst>
 </file>
@@ -357,16 +357,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -669,160 +666,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.53125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.46484375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.9296875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="3.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>8.5</v>
+      </c>
+      <c r="F2">
         <v>9</v>
       </c>
-      <c r="D2">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="E2">
-        <v>7.8</v>
-      </c>
-      <c r="F2">
-        <v>8.5</v>
-      </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="D3">
-        <v>17.2</v>
+        <v>16</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>4.5</v>
       </c>
       <c r="F3">
-        <v>8.8000000000000007</v>
+        <v>2.5</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="D4">
         <v>17</v>
       </c>
       <c r="E4">
-        <v>8.5</v>
+        <v>4.5</v>
       </c>
       <c r="F4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>17.5</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>6.5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6">
-        <v>18</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G4">
+    <sortCondition ref="A1:A4"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -845,82 +799,82 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <v>18.2</v>
       </c>
       <c r="E2">
-        <v>8.5</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F2">
-        <v>8.5</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>8.5</v>
+      </c>
+      <c r="F3">
+        <v>8.5</v>
+      </c>
+      <c r="G3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3">
-        <v>18.2</v>
-      </c>
-      <c r="E3">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="F3">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>18.3</v>
@@ -932,18 +886,18 @@
         <v>7.8</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>18</v>
@@ -955,15 +909,180 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G5">
+    <sortCondition ref="A1:A5"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="30.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="3.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>8.5</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E3">
+        <v>7.8</v>
+      </c>
+      <c r="F3">
+        <v>8.5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>17.2</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>17.5</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>6.5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G6">
+    <sortCondition ref="A1:A6"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -982,82 +1101,82 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <v>18.3</v>
       </c>
       <c r="E2">
-        <v>8.5</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>8.5</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3">
-        <v>18.3</v>
-      </c>
-      <c r="E3">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="F3">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>17.5</v>
@@ -1069,15 +1188,157 @@
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G4">
+    <sortCondition ref="A1:A4"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E2">
+        <v>6.5</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5">
+        <v>16.7</v>
+      </c>
+      <c r="E5">
+        <v>10.4</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G5">
+    <sortCondition ref="A1:A5"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1096,346 +1357,100 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>5.5</v>
       </c>
       <c r="F2">
-        <v>10.5</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>10.5</v>
+      </c>
+      <c r="G3" t="s">
         <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3">
-        <v>17.5</v>
-      </c>
-      <c r="E3">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D4">
-        <v>16</v>
+        <v>17.5</v>
       </c>
       <c r="E4">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="18.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="3.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.1328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2">
-        <v>17</v>
-      </c>
-      <c r="E2">
-        <v>4.5</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>4.5</v>
-      </c>
-      <c r="F3">
-        <v>2.5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4">
-        <v>18</v>
-      </c>
-      <c r="E4">
-        <v>8.5</v>
-      </c>
-      <c r="F4">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="4.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.9296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.73046875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3">
-        <v>16.7</v>
-      </c>
-      <c r="E3">
-        <v>10.4</v>
-      </c>
-      <c r="F3">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4">
-        <v>16</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="E5">
-        <v>6.5</v>
-      </c>
-      <c r="F5">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G4">
+    <sortCondition ref="A1:A4"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1459,82 +1474,82 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D2">
-        <v>17</v>
+        <v>18.5</v>
       </c>
       <c r="E2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D3">
         <v>17</v>
       </c>
       <c r="E3">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D4">
         <v>18</v>
@@ -1546,33 +1561,36 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D5">
-        <v>18.5</v>
+        <v>17</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G5">
+    <sortCondition ref="A1:A5"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>